<commit_message>
Updated Tree and plan
</commit_message>
<xml_diff>
--- a/Integrationsplan.xlsx
+++ b/Integrationsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trill\OneDrive\Skrivebord\SWT SOURCE\Microwave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAF31CB-44FF-4EE4-BEE1-DA7567D48EFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821C3242-4C41-4AF5-97D6-C84546D6B8A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{87B4455E-598E-4405-AA2E-7FB99C6EE422}"/>
   </bookViews>
@@ -821,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB7CB98-BA48-456B-A21B-B60D1F434C44}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new integration plan, hopefully final
</commit_message>
<xml_diff>
--- a/Integrationsplan.xlsx
+++ b/Integrationsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trill\OneDrive\Skrivebord\SWT SOURCE\Microwave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75BDDF0-92D6-4D9F-9237-37C4AA909AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC32886-FECA-4B62-BC7F-165908A70B1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{87B4455E-598E-4405-AA2E-7FB99C6EE422}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="17">
   <si>
     <t>Step #</t>
   </si>
@@ -79,12 +79,15 @@
   <si>
     <t>Tiers</t>
   </si>
+  <si>
+    <t>RIGTIG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +119,12 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -444,11 +453,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -478,7 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -491,6 +605,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB7CB98-BA48-456B-A21B-B60D1F434C44}">
-  <dimension ref="A1:AH43"/>
+  <dimension ref="A1:AH55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG19" sqref="AG19"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,10 +1033,10 @@
       <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
@@ -919,9 +1047,15 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
@@ -936,51 +1070,57 @@
       <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33">
+      <c r="L2" s="32"/>
+      <c r="M2" s="32">
         <v>1</v>
       </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="X2" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD2" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE2" s="38"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="37"/>
     </row>
     <row r="3" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
@@ -999,47 +1139,51 @@
       <c r="M3" s="24">
         <v>1</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="X3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y3" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z3" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA3" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB3" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC3" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD3" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE3" s="38"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD3" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="37"/>
     </row>
     <row r="4" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1058,621 +1202,541 @@
       <c r="K4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33">
+      <c r="L4" s="32"/>
+      <c r="M4" s="32">
         <v>1</v>
       </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="X4" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE4" s="38" t="s">
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="X4" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD4" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE4" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11">
+      <c r="A5" s="45">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25">
+      <c r="B5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47">
         <v>1</v>
       </c>
-      <c r="N5" s="37"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="X5" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y5" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z5" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA5" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB5" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC5" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD5" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE5" s="38" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="N5" s="36"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE5" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="42">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="33">
+      <c r="B6" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="43"/>
+      <c r="M6" s="44">
         <v>2</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="39"/>
-      <c r="AC6" s="39"/>
-      <c r="AD6" s="39"/>
-      <c r="AE6" s="39"/>
-    </row>
-    <row r="7" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+    </row>
+    <row r="7" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="49">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="24">
-        <v>2</v>
-      </c>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="39"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="39"/>
-      <c r="X7" s="39"/>
-      <c r="Y7" s="39"/>
-      <c r="Z7" s="39"/>
-      <c r="AA7" s="39"/>
-      <c r="AB7" s="39"/>
-      <c r="AC7" s="39"/>
-      <c r="AD7" s="39"/>
-      <c r="AE7" s="39"/>
+      <c r="B7" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="50"/>
+      <c r="M7" s="51">
+        <v>3</v>
+      </c>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="38"/>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="38"/>
     </row>
     <row r="8" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="33">
-        <v>2</v>
-      </c>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="X8" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y8" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD8" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE8" s="38"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="48">
+        <v>4</v>
+      </c>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="X8" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y8" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="37"/>
+      <c r="AB8" s="37"/>
+      <c r="AC8" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD8" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE8" s="37"/>
     </row>
     <row r="9" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
+      <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="12"/>
-      <c r="M9" s="12">
-        <v>2</v>
-      </c>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="X9" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y9" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z9" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA9" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB9" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC9" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD9" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE9" s="38"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="X9" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y9" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE9" s="37"/>
     </row>
     <row r="10" spans="1:31" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="33">
-        <v>3</v>
-      </c>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="X10" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y10" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z10" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA10" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB10" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC10" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD10" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE10" s="38" t="s">
+      <c r="M10" s="32"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="X10" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y10" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z10" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA10" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB10" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC10" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD10" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE10" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="30"/>
-      <c r="M11" s="24">
-        <v>3</v>
-      </c>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="X11" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y11" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z11" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA11" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB11" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC11" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD11" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE11" s="38" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="X11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA11" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC11" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE11" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
+      <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="33">
-        <v>3</v>
-      </c>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="X12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA12" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE12" s="38" t="s">
+      <c r="M12" s="32"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB12" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD12" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE12" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
+      <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="12"/>
-      <c r="M13" s="12">
-        <v>3</v>
-      </c>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="X13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA13" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE13" s="38"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="X13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE13" s="37"/>
     </row>
     <row r="14" spans="1:31" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13">
@@ -1702,40 +1766,40 @@
       <c r="M14" s="14">
         <v>4</v>
       </c>
-      <c r="N14" s="40"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="X14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD14" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE14" s="41" t="s">
+      <c r="N14" s="39"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="X14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD14" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE14" s="40" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1765,8 +1829,8 @@
       <c r="K15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31">
+      <c r="L15" s="30"/>
+      <c r="M15" s="30">
         <v>5</v>
       </c>
       <c r="N15" s="26"/>
@@ -1800,7 +1864,7 @@
         <v>10</v>
       </c>
       <c r="L16" s="21"/>
-      <c r="M16" s="33">
+      <c r="M16" s="32">
         <v>6</v>
       </c>
       <c r="N16" s="26"/>
@@ -1815,25 +1879,25 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="32"/>
+      <c r="F17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="31"/>
       <c r="M17" s="24">
         <v>6</v>
       </c>
@@ -1868,7 +1932,7 @@
         <v>10</v>
       </c>
       <c r="L18" s="22"/>
-      <c r="M18" s="33">
+      <c r="M18" s="32">
         <v>6</v>
       </c>
       <c r="N18" s="26"/>
@@ -1905,7 +1969,7 @@
       <c r="M19" s="25">
         <v>6</v>
       </c>
-      <c r="N19" s="35"/>
+      <c r="N19" s="34"/>
     </row>
     <row r="20" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
@@ -1938,7 +2002,7 @@
       <c r="L20" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="33">
+      <c r="M20" s="32">
         <v>7</v>
       </c>
       <c r="N20" s="26"/>
@@ -1953,25 +2017,25 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="32" t="s">
+      <c r="F21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="31" t="s">
         <v>10</v>
       </c>
       <c r="M21" s="24">
@@ -2010,7 +2074,7 @@
       <c r="L22" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="33">
+      <c r="M22" s="32">
         <v>7</v>
       </c>
       <c r="N22" s="28"/>
@@ -2082,7 +2146,7 @@
       <c r="L24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M24" s="33">
+      <c r="M24" s="32">
         <v>8</v>
       </c>
       <c r="N24" s="28"/>
@@ -2154,7 +2218,7 @@
       <c r="L26" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="M26" s="33">
+      <c r="M26" s="32">
         <v>8</v>
       </c>
       <c r="N26" s="28"/>
@@ -2226,7 +2290,7 @@
       <c r="L28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M28" s="33">
+      <c r="M28" s="32">
         <v>9</v>
       </c>
       <c r="N28" s="28"/>
@@ -2298,7 +2362,7 @@
       <c r="L30" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="M30" s="33">
+      <c r="M30" s="32">
         <v>9</v>
       </c>
       <c r="N30" s="28"/>
@@ -2367,10 +2431,10 @@
       <c r="K32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M32" s="33">
+      <c r="L32" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" s="32">
         <v>10</v>
       </c>
       <c r="N32" s="26"/>
@@ -2434,7 +2498,7 @@
       <c r="AF33" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AG33" s="34" t="s">
+      <c r="AG33" s="33" t="s">
         <v>11</v>
       </c>
       <c r="AH33" s="24">
@@ -2469,10 +2533,10 @@
       <c r="K34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L34" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M34" s="33">
+      <c r="L34" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" s="32">
         <v>10</v>
       </c>
       <c r="N34" s="26"/>
@@ -2593,10 +2657,12 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:34" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:34" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A41" s="27"/>
       <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
+      <c r="C41" s="54" t="s">
+        <v>16</v>
+      </c>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
       <c r="F41" s="28"/>
@@ -2609,25 +2675,505 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:34" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
+    <row r="42" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L42" s="35" t="s">
+        <v>8</v>
+      </c>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
     </row>
-    <row r="43" spans="1:34" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L43" s="32"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L44" s="24"/>
+    </row>
+    <row r="45" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="32"/>
+    </row>
+    <row r="46" spans="1:34" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="45">
+        <v>1</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="K46" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="47"/>
+    </row>
+    <row r="47" spans="1:34" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="49">
+        <v>2</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="K47" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="43"/>
+    </row>
+    <row r="48" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="8">
+        <v>3</v>
+      </c>
+      <c r="B48" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J48" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="K48" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="L48" s="52"/>
+    </row>
+    <row r="49" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="45">
+        <v>3</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="K49" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="L49" s="53"/>
+    </row>
+    <row r="50" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="8">
+        <v>4</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="L50" s="41"/>
+    </row>
+    <row r="51" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="45">
+        <v>4</v>
+      </c>
+      <c r="B51" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I51" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="K51" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="L51" s="53"/>
+    </row>
+    <row r="52" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="8">
+        <v>5</v>
+      </c>
+      <c r="B52" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="K52" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="L52" s="41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>6</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>7</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="45">
+        <v>8</v>
+      </c>
+      <c r="B55" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="K55" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="L55" s="53" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>